<commit_message>
Chỉnh sửa lại một vài lỗi
</commit_message>
<xml_diff>
--- a/public/templates/bai_thi_template.xlsx
+++ b/public/templates/bai_thi_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dowload\DL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Khoa_luan\thi_trac_nghiem_truc_tuyen\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A64292-E557-4B32-8231-F6C19EA96FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F371B8-E508-4D8A-A166-E1811B94ABB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D9A8524-71F9-4E97-BEE1-1E68B6DB1399}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Mã bài thi</t>
   </si>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>Thí sinh chỉ được dùng một thiết bị. Không được sử dụng tài liệu trong quá trình làm bài. Phải làm bài bằng VLU THI.</t>
+  </si>
+  <si>
+    <t>Mã lớp học phần</t>
+  </si>
+  <si>
+    <t>LHP_PTNC</t>
+  </si>
+  <si>
+    <t>LHP_CSDL</t>
+  </si>
+  <si>
+    <t>LHP_LTLN</t>
   </si>
 </sst>
 </file>
@@ -583,89 +595,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05FCAC7-8C9C-4D8B-B5EA-64CCEBA17FA9}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="27" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="29.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.28515625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cập nhật chức năng
</commit_message>
<xml_diff>
--- a/public/templates/bai_thi_template.xlsx
+++ b/public/templates/bai_thi_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Khoa_luan\thi_trac_nghiem_truc_tuyen\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F371B8-E508-4D8A-A166-E1811B94ABB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A0F852-A113-4803-924C-D04DA8FEDE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1D9A8524-71F9-4E97-BEE1-1E68B6DB1399}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Mã bài thi</t>
   </si>
@@ -102,6 +102,21 @@
   </si>
   <si>
     <t>LHP_LTLN</t>
+  </si>
+  <si>
+    <t>Mã môn học</t>
+  </si>
+  <si>
+    <t>Lần thi</t>
+  </si>
+  <si>
+    <t>LTPY</t>
+  </si>
+  <si>
+    <t>CSDL</t>
+  </si>
+  <si>
+    <t>LN</t>
   </si>
 </sst>
 </file>
@@ -595,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05FCAC7-8C9C-4D8B-B5EA-64CCEBA17FA9}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +629,7 @@
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -622,19 +637,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -642,19 +663,25 @@
         <v>5</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="8">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -662,19 +689,25 @@
         <v>7</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="8">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -682,15 +715,21 @@
         <v>9</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="8">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>